<commit_message>
Update Lista de itens e riscos
</commit_message>
<xml_diff>
--- a/planejamento/CM_Lista_riscos.xlsx
+++ b/planejamento/CM_Lista_riscos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Riscos" sheetId="1" state="visible" r:id="rId2"/>
@@ -181,14 +181,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="[$R$-416]\ #,##0.00;[RED]\-[$R$-416]\ #,##0.00"/>
-    <numFmt numFmtId="166" formatCode="D/M/YYYY"/>
-    <numFmt numFmtId="167" formatCode="0%"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="D/M/YYYY"/>
+    <numFmt numFmtId="166" formatCode="0%"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -210,25 +209,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <sz val="16"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -306,7 +286,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="24">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -329,28 +309,12 @@
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -359,94 +323,78 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading 1" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading1 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Result 1" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Result2 1" xfId="23" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -518,7 +466,7 @@
   </sheetPr>
   <dimension ref="A1:IW26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -851,11 +799,11 @@
         <v>5</v>
       </c>
       <c r="G3" s="8" t="n">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="H3" s="9" t="n">
         <f aca="false">+F3*G3</f>
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>14</v>
@@ -897,7 +845,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" s="11" customFormat="true" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="11" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="n">
         <v>3</v>
       </c>
@@ -917,11 +865,11 @@
         <v>2</v>
       </c>
       <c r="G5" s="8" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="H5" s="9" t="n">
         <f aca="false">+F5*G5</f>
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="I5" s="9" t="s">
         <v>14</v>
@@ -950,11 +898,11 @@
         <v>4</v>
       </c>
       <c r="G6" s="8" t="n">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="H6" s="9" t="n">
         <f aca="false">+F6*G6</f>
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="I6" s="9" t="s">
         <v>14</v>
@@ -1035,11 +983,11 @@
         <v>8</v>
       </c>
       <c r="B10" s="7"/>
-      <c r="C10" s="12"/>
+      <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="13"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="12"/>
       <c r="H10" s="9" t="n">
         <f aca="false">+F10*G10</f>
         <v>0</v>
@@ -1069,11 +1017,11 @@
         <v>10</v>
       </c>
       <c r="B12" s="7"/>
-      <c r="C12" s="12"/>
+      <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="14"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="8"/>
       <c r="H12" s="9" t="n">
         <f aca="false">+F12*G12</f>
         <v>0</v>
@@ -1085,29 +1033,29 @@
       <c r="A13" s="6" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="18"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="15"/>
       <c r="H13" s="9" t="n">
         <f aca="false">+F13*G13</f>
         <v>0</v>
       </c>
-      <c r="I13" s="19"/>
-      <c r="J13" s="20"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="17"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="n">
         <v>12</v>
       </c>
       <c r="B14" s="7"/>
-      <c r="C14" s="12"/>
+      <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="13"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="12"/>
       <c r="H14" s="9" t="n">
         <f aca="false">+F14*G14</f>
         <v>0</v>
@@ -1137,11 +1085,11 @@
         <v>14</v>
       </c>
       <c r="B16" s="7"/>
-      <c r="C16" s="12"/>
+      <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="14"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="8"/>
       <c r="H16" s="9" t="n">
         <f aca="false">+F16*G16</f>
         <v>0</v>
@@ -1205,11 +1153,11 @@
         <v>18</v>
       </c>
       <c r="B20" s="7"/>
-      <c r="C20" s="12"/>
+      <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="14"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="8"/>
       <c r="H20" s="9" t="n">
         <f aca="false">+F20*G20</f>
         <v>0</v>

</xml_diff>

<commit_message>
redução dos riscos do projeto
</commit_message>
<xml_diff>
--- a/planejamento/CM_Lista_riscos.xlsx
+++ b/planejamento/CM_Lista_riscos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Riscos" sheetId="1" state="visible" r:id="rId2"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Lista de Riscos: Projeto Car Management Project</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>Faculdade não dispõe de internet capaz de enviar as entregas ao repositório no dia. E viagens de integrantes da equipe para locais sem acesso a internet.</t>
+  </si>
+  <si>
+    <t>Tarcísio, Diógenes</t>
   </si>
   <si>
     <t>Enviar as entregas com antecedência em local que disponha de internet.</t>
@@ -235,6 +238,7 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -242,7 +246,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -328,71 +331,71 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -473,25 +476,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="1:26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.32093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.8883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="34.2093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="34.9488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="3.56744186046512"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="3.32093023255814"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="6.89302325581395"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="3.81395348837209"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.2"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="35.3209302325581"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3.56744186046512"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.6279069767442"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.3023255813953"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="37.0418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="3.81395348837209"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="3.56744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.13953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="4.06046511627907"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.9348837209302"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="37.4093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -507,6 +510,1020 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
+      <c r="K1" s="0"/>
+      <c r="L1" s="0"/>
+      <c r="M1" s="0"/>
+      <c r="N1" s="0"/>
+      <c r="O1" s="0"/>
+      <c r="P1" s="0"/>
+      <c r="Q1" s="0"/>
+      <c r="R1" s="0"/>
+      <c r="S1" s="0"/>
+      <c r="T1" s="0"/>
+      <c r="U1" s="0"/>
+      <c r="V1" s="0"/>
+      <c r="W1" s="0"/>
+      <c r="X1" s="0"/>
+      <c r="Y1" s="0"/>
+      <c r="Z1" s="0"/>
+      <c r="AA1" s="0"/>
+      <c r="AB1" s="0"/>
+      <c r="AC1" s="0"/>
+      <c r="AD1" s="0"/>
+      <c r="AE1" s="0"/>
+      <c r="AF1" s="0"/>
+      <c r="AG1" s="0"/>
+      <c r="AH1" s="0"/>
+      <c r="AI1" s="0"/>
+      <c r="AJ1" s="0"/>
+      <c r="AK1" s="0"/>
+      <c r="AL1" s="0"/>
+      <c r="AM1" s="0"/>
+      <c r="AN1" s="0"/>
+      <c r="AO1" s="0"/>
+      <c r="AP1" s="0"/>
+      <c r="AQ1" s="0"/>
+      <c r="AR1" s="0"/>
+      <c r="AS1" s="0"/>
+      <c r="AT1" s="0"/>
+      <c r="AU1" s="0"/>
+      <c r="AV1" s="0"/>
+      <c r="AW1" s="0"/>
+      <c r="AX1" s="0"/>
+      <c r="AY1" s="0"/>
+      <c r="AZ1" s="0"/>
+      <c r="BA1" s="0"/>
+      <c r="BB1" s="0"/>
+      <c r="BC1" s="0"/>
+      <c r="BD1" s="0"/>
+      <c r="BE1" s="0"/>
+      <c r="BF1" s="0"/>
+      <c r="BG1" s="0"/>
+      <c r="BH1" s="0"/>
+      <c r="BI1" s="0"/>
+      <c r="BJ1" s="0"/>
+      <c r="BK1" s="0"/>
+      <c r="BL1" s="0"/>
+      <c r="BM1" s="0"/>
+      <c r="BN1" s="0"/>
+      <c r="BO1" s="0"/>
+      <c r="BP1" s="0"/>
+      <c r="BQ1" s="0"/>
+      <c r="BR1" s="0"/>
+      <c r="BS1" s="0"/>
+      <c r="BT1" s="0"/>
+      <c r="BU1" s="0"/>
+      <c r="BV1" s="0"/>
+      <c r="BW1" s="0"/>
+      <c r="BX1" s="0"/>
+      <c r="BY1" s="0"/>
+      <c r="BZ1" s="0"/>
+      <c r="CA1" s="0"/>
+      <c r="CB1" s="0"/>
+      <c r="CC1" s="0"/>
+      <c r="CD1" s="0"/>
+      <c r="CE1" s="0"/>
+      <c r="CF1" s="0"/>
+      <c r="CG1" s="0"/>
+      <c r="CH1" s="0"/>
+      <c r="CI1" s="0"/>
+      <c r="CJ1" s="0"/>
+      <c r="CK1" s="0"/>
+      <c r="CL1" s="0"/>
+      <c r="CM1" s="0"/>
+      <c r="CN1" s="0"/>
+      <c r="CO1" s="0"/>
+      <c r="CP1" s="0"/>
+      <c r="CQ1" s="0"/>
+      <c r="CR1" s="0"/>
+      <c r="CS1" s="0"/>
+      <c r="CT1" s="0"/>
+      <c r="CU1" s="0"/>
+      <c r="CV1" s="0"/>
+      <c r="CW1" s="0"/>
+      <c r="CX1" s="0"/>
+      <c r="CY1" s="0"/>
+      <c r="CZ1" s="0"/>
+      <c r="DA1" s="0"/>
+      <c r="DB1" s="0"/>
+      <c r="DC1" s="0"/>
+      <c r="DD1" s="0"/>
+      <c r="DE1" s="0"/>
+      <c r="DF1" s="0"/>
+      <c r="DG1" s="0"/>
+      <c r="DH1" s="0"/>
+      <c r="DI1" s="0"/>
+      <c r="DJ1" s="0"/>
+      <c r="DK1" s="0"/>
+      <c r="DL1" s="0"/>
+      <c r="DM1" s="0"/>
+      <c r="DN1" s="0"/>
+      <c r="DO1" s="0"/>
+      <c r="DP1" s="0"/>
+      <c r="DQ1" s="0"/>
+      <c r="DR1" s="0"/>
+      <c r="DS1" s="0"/>
+      <c r="DT1" s="0"/>
+      <c r="DU1" s="0"/>
+      <c r="DV1" s="0"/>
+      <c r="DW1" s="0"/>
+      <c r="DX1" s="0"/>
+      <c r="DY1" s="0"/>
+      <c r="DZ1" s="0"/>
+      <c r="EA1" s="0"/>
+      <c r="EB1" s="0"/>
+      <c r="EC1" s="0"/>
+      <c r="ED1" s="0"/>
+      <c r="EE1" s="0"/>
+      <c r="EF1" s="0"/>
+      <c r="EG1" s="0"/>
+      <c r="EH1" s="0"/>
+      <c r="EI1" s="0"/>
+      <c r="EJ1" s="0"/>
+      <c r="EK1" s="0"/>
+      <c r="EL1" s="0"/>
+      <c r="EM1" s="0"/>
+      <c r="EN1" s="0"/>
+      <c r="EO1" s="0"/>
+      <c r="EP1" s="0"/>
+      <c r="EQ1" s="0"/>
+      <c r="ER1" s="0"/>
+      <c r="ES1" s="0"/>
+      <c r="ET1" s="0"/>
+      <c r="EU1" s="0"/>
+      <c r="EV1" s="0"/>
+      <c r="EW1" s="0"/>
+      <c r="EX1" s="0"/>
+      <c r="EY1" s="0"/>
+      <c r="EZ1" s="0"/>
+      <c r="FA1" s="0"/>
+      <c r="FB1" s="0"/>
+      <c r="FC1" s="0"/>
+      <c r="FD1" s="0"/>
+      <c r="FE1" s="0"/>
+      <c r="FF1" s="0"/>
+      <c r="FG1" s="0"/>
+      <c r="FH1" s="0"/>
+      <c r="FI1" s="0"/>
+      <c r="FJ1" s="0"/>
+      <c r="FK1" s="0"/>
+      <c r="FL1" s="0"/>
+      <c r="FM1" s="0"/>
+      <c r="FN1" s="0"/>
+      <c r="FO1" s="0"/>
+      <c r="FP1" s="0"/>
+      <c r="FQ1" s="0"/>
+      <c r="FR1" s="0"/>
+      <c r="FS1" s="0"/>
+      <c r="FT1" s="0"/>
+      <c r="FU1" s="0"/>
+      <c r="FV1" s="0"/>
+      <c r="FW1" s="0"/>
+      <c r="FX1" s="0"/>
+      <c r="FY1" s="0"/>
+      <c r="FZ1" s="0"/>
+      <c r="GA1" s="0"/>
+      <c r="GB1" s="0"/>
+      <c r="GC1" s="0"/>
+      <c r="GD1" s="0"/>
+      <c r="GE1" s="0"/>
+      <c r="GF1" s="0"/>
+      <c r="GG1" s="0"/>
+      <c r="GH1" s="0"/>
+      <c r="GI1" s="0"/>
+      <c r="GJ1" s="0"/>
+      <c r="GK1" s="0"/>
+      <c r="GL1" s="0"/>
+      <c r="GM1" s="0"/>
+      <c r="GN1" s="0"/>
+      <c r="GO1" s="0"/>
+      <c r="GP1" s="0"/>
+      <c r="GQ1" s="0"/>
+      <c r="GR1" s="0"/>
+      <c r="GS1" s="0"/>
+      <c r="GT1" s="0"/>
+      <c r="GU1" s="0"/>
+      <c r="GV1" s="0"/>
+      <c r="GW1" s="0"/>
+      <c r="GX1" s="0"/>
+      <c r="GY1" s="0"/>
+      <c r="GZ1" s="0"/>
+      <c r="HA1" s="0"/>
+      <c r="HB1" s="0"/>
+      <c r="HC1" s="0"/>
+      <c r="HD1" s="0"/>
+      <c r="HE1" s="0"/>
+      <c r="HF1" s="0"/>
+      <c r="HG1" s="0"/>
+      <c r="HH1" s="0"/>
+      <c r="HI1" s="0"/>
+      <c r="HJ1" s="0"/>
+      <c r="HK1" s="0"/>
+      <c r="HL1" s="0"/>
+      <c r="HM1" s="0"/>
+      <c r="HN1" s="0"/>
+      <c r="HO1" s="0"/>
+      <c r="HP1" s="0"/>
+      <c r="HQ1" s="0"/>
+      <c r="HR1" s="0"/>
+      <c r="HS1" s="0"/>
+      <c r="HT1" s="0"/>
+      <c r="HU1" s="0"/>
+      <c r="HV1" s="0"/>
+      <c r="HW1" s="0"/>
+      <c r="HX1" s="0"/>
+      <c r="HY1" s="0"/>
+      <c r="HZ1" s="0"/>
+      <c r="IA1" s="0"/>
+      <c r="IB1" s="0"/>
+      <c r="IC1" s="0"/>
+      <c r="ID1" s="0"/>
+      <c r="IE1" s="0"/>
+      <c r="IF1" s="0"/>
+      <c r="IG1" s="0"/>
+      <c r="IH1" s="0"/>
+      <c r="II1" s="0"/>
+      <c r="IJ1" s="0"/>
+      <c r="IK1" s="0"/>
+      <c r="IL1" s="0"/>
+      <c r="IM1" s="0"/>
+      <c r="IN1" s="0"/>
+      <c r="IO1" s="0"/>
+      <c r="IP1" s="0"/>
+      <c r="IQ1" s="0"/>
+      <c r="IR1" s="0"/>
+      <c r="IS1" s="0"/>
+      <c r="IT1" s="0"/>
+      <c r="IU1" s="0"/>
+      <c r="IV1" s="0"/>
+      <c r="IW1" s="0"/>
+      <c r="IX1" s="0"/>
+      <c r="IY1" s="0"/>
+      <c r="IZ1" s="0"/>
+      <c r="JA1" s="0"/>
+      <c r="JB1" s="0"/>
+      <c r="JC1" s="0"/>
+      <c r="JD1" s="0"/>
+      <c r="JE1" s="0"/>
+      <c r="JF1" s="0"/>
+      <c r="JG1" s="0"/>
+      <c r="JH1" s="0"/>
+      <c r="JI1" s="0"/>
+      <c r="JJ1" s="0"/>
+      <c r="JK1" s="0"/>
+      <c r="JL1" s="0"/>
+      <c r="JM1" s="0"/>
+      <c r="JN1" s="0"/>
+      <c r="JO1" s="0"/>
+      <c r="JP1" s="0"/>
+      <c r="JQ1" s="0"/>
+      <c r="JR1" s="0"/>
+      <c r="JS1" s="0"/>
+      <c r="JT1" s="0"/>
+      <c r="JU1" s="0"/>
+      <c r="JV1" s="0"/>
+      <c r="JW1" s="0"/>
+      <c r="JX1" s="0"/>
+      <c r="JY1" s="0"/>
+      <c r="JZ1" s="0"/>
+      <c r="KA1" s="0"/>
+      <c r="KB1" s="0"/>
+      <c r="KC1" s="0"/>
+      <c r="KD1" s="0"/>
+      <c r="KE1" s="0"/>
+      <c r="KF1" s="0"/>
+      <c r="KG1" s="0"/>
+      <c r="KH1" s="0"/>
+      <c r="KI1" s="0"/>
+      <c r="KJ1" s="0"/>
+      <c r="KK1" s="0"/>
+      <c r="KL1" s="0"/>
+      <c r="KM1" s="0"/>
+      <c r="KN1" s="0"/>
+      <c r="KO1" s="0"/>
+      <c r="KP1" s="0"/>
+      <c r="KQ1" s="0"/>
+      <c r="KR1" s="0"/>
+      <c r="KS1" s="0"/>
+      <c r="KT1" s="0"/>
+      <c r="KU1" s="0"/>
+      <c r="KV1" s="0"/>
+      <c r="KW1" s="0"/>
+      <c r="KX1" s="0"/>
+      <c r="KY1" s="0"/>
+      <c r="KZ1" s="0"/>
+      <c r="LA1" s="0"/>
+      <c r="LB1" s="0"/>
+      <c r="LC1" s="0"/>
+      <c r="LD1" s="0"/>
+      <c r="LE1" s="0"/>
+      <c r="LF1" s="0"/>
+      <c r="LG1" s="0"/>
+      <c r="LH1" s="0"/>
+      <c r="LI1" s="0"/>
+      <c r="LJ1" s="0"/>
+      <c r="LK1" s="0"/>
+      <c r="LL1" s="0"/>
+      <c r="LM1" s="0"/>
+      <c r="LN1" s="0"/>
+      <c r="LO1" s="0"/>
+      <c r="LP1" s="0"/>
+      <c r="LQ1" s="0"/>
+      <c r="LR1" s="0"/>
+      <c r="LS1" s="0"/>
+      <c r="LT1" s="0"/>
+      <c r="LU1" s="0"/>
+      <c r="LV1" s="0"/>
+      <c r="LW1" s="0"/>
+      <c r="LX1" s="0"/>
+      <c r="LY1" s="0"/>
+      <c r="LZ1" s="0"/>
+      <c r="MA1" s="0"/>
+      <c r="MB1" s="0"/>
+      <c r="MC1" s="0"/>
+      <c r="MD1" s="0"/>
+      <c r="ME1" s="0"/>
+      <c r="MF1" s="0"/>
+      <c r="MG1" s="0"/>
+      <c r="MH1" s="0"/>
+      <c r="MI1" s="0"/>
+      <c r="MJ1" s="0"/>
+      <c r="MK1" s="0"/>
+      <c r="ML1" s="0"/>
+      <c r="MM1" s="0"/>
+      <c r="MN1" s="0"/>
+      <c r="MO1" s="0"/>
+      <c r="MP1" s="0"/>
+      <c r="MQ1" s="0"/>
+      <c r="MR1" s="0"/>
+      <c r="MS1" s="0"/>
+      <c r="MT1" s="0"/>
+      <c r="MU1" s="0"/>
+      <c r="MV1" s="0"/>
+      <c r="MW1" s="0"/>
+      <c r="MX1" s="0"/>
+      <c r="MY1" s="0"/>
+      <c r="MZ1" s="0"/>
+      <c r="NA1" s="0"/>
+      <c r="NB1" s="0"/>
+      <c r="NC1" s="0"/>
+      <c r="ND1" s="0"/>
+      <c r="NE1" s="0"/>
+      <c r="NF1" s="0"/>
+      <c r="NG1" s="0"/>
+      <c r="NH1" s="0"/>
+      <c r="NI1" s="0"/>
+      <c r="NJ1" s="0"/>
+      <c r="NK1" s="0"/>
+      <c r="NL1" s="0"/>
+      <c r="NM1" s="0"/>
+      <c r="NN1" s="0"/>
+      <c r="NO1" s="0"/>
+      <c r="NP1" s="0"/>
+      <c r="NQ1" s="0"/>
+      <c r="NR1" s="0"/>
+      <c r="NS1" s="0"/>
+      <c r="NT1" s="0"/>
+      <c r="NU1" s="0"/>
+      <c r="NV1" s="0"/>
+      <c r="NW1" s="0"/>
+      <c r="NX1" s="0"/>
+      <c r="NY1" s="0"/>
+      <c r="NZ1" s="0"/>
+      <c r="OA1" s="0"/>
+      <c r="OB1" s="0"/>
+      <c r="OC1" s="0"/>
+      <c r="OD1" s="0"/>
+      <c r="OE1" s="0"/>
+      <c r="OF1" s="0"/>
+      <c r="OG1" s="0"/>
+      <c r="OH1" s="0"/>
+      <c r="OI1" s="0"/>
+      <c r="OJ1" s="0"/>
+      <c r="OK1" s="0"/>
+      <c r="OL1" s="0"/>
+      <c r="OM1" s="0"/>
+      <c r="ON1" s="0"/>
+      <c r="OO1" s="0"/>
+      <c r="OP1" s="0"/>
+      <c r="OQ1" s="0"/>
+      <c r="OR1" s="0"/>
+      <c r="OS1" s="0"/>
+      <c r="OT1" s="0"/>
+      <c r="OU1" s="0"/>
+      <c r="OV1" s="0"/>
+      <c r="OW1" s="0"/>
+      <c r="OX1" s="0"/>
+      <c r="OY1" s="0"/>
+      <c r="OZ1" s="0"/>
+      <c r="PA1" s="0"/>
+      <c r="PB1" s="0"/>
+      <c r="PC1" s="0"/>
+      <c r="PD1" s="0"/>
+      <c r="PE1" s="0"/>
+      <c r="PF1" s="0"/>
+      <c r="PG1" s="0"/>
+      <c r="PH1" s="0"/>
+      <c r="PI1" s="0"/>
+      <c r="PJ1" s="0"/>
+      <c r="PK1" s="0"/>
+      <c r="PL1" s="0"/>
+      <c r="PM1" s="0"/>
+      <c r="PN1" s="0"/>
+      <c r="PO1" s="0"/>
+      <c r="PP1" s="0"/>
+      <c r="PQ1" s="0"/>
+      <c r="PR1" s="0"/>
+      <c r="PS1" s="0"/>
+      <c r="PT1" s="0"/>
+      <c r="PU1" s="0"/>
+      <c r="PV1" s="0"/>
+      <c r="PW1" s="0"/>
+      <c r="PX1" s="0"/>
+      <c r="PY1" s="0"/>
+      <c r="PZ1" s="0"/>
+      <c r="QA1" s="0"/>
+      <c r="QB1" s="0"/>
+      <c r="QC1" s="0"/>
+      <c r="QD1" s="0"/>
+      <c r="QE1" s="0"/>
+      <c r="QF1" s="0"/>
+      <c r="QG1" s="0"/>
+      <c r="QH1" s="0"/>
+      <c r="QI1" s="0"/>
+      <c r="QJ1" s="0"/>
+      <c r="QK1" s="0"/>
+      <c r="QL1" s="0"/>
+      <c r="QM1" s="0"/>
+      <c r="QN1" s="0"/>
+      <c r="QO1" s="0"/>
+      <c r="QP1" s="0"/>
+      <c r="QQ1" s="0"/>
+      <c r="QR1" s="0"/>
+      <c r="QS1" s="0"/>
+      <c r="QT1" s="0"/>
+      <c r="QU1" s="0"/>
+      <c r="QV1" s="0"/>
+      <c r="QW1" s="0"/>
+      <c r="QX1" s="0"/>
+      <c r="QY1" s="0"/>
+      <c r="QZ1" s="0"/>
+      <c r="RA1" s="0"/>
+      <c r="RB1" s="0"/>
+      <c r="RC1" s="0"/>
+      <c r="RD1" s="0"/>
+      <c r="RE1" s="0"/>
+      <c r="RF1" s="0"/>
+      <c r="RG1" s="0"/>
+      <c r="RH1" s="0"/>
+      <c r="RI1" s="0"/>
+      <c r="RJ1" s="0"/>
+      <c r="RK1" s="0"/>
+      <c r="RL1" s="0"/>
+      <c r="RM1" s="0"/>
+      <c r="RN1" s="0"/>
+      <c r="RO1" s="0"/>
+      <c r="RP1" s="0"/>
+      <c r="RQ1" s="0"/>
+      <c r="RR1" s="0"/>
+      <c r="RS1" s="0"/>
+      <c r="RT1" s="0"/>
+      <c r="RU1" s="0"/>
+      <c r="RV1" s="0"/>
+      <c r="RW1" s="0"/>
+      <c r="RX1" s="0"/>
+      <c r="RY1" s="0"/>
+      <c r="RZ1" s="0"/>
+      <c r="SA1" s="0"/>
+      <c r="SB1" s="0"/>
+      <c r="SC1" s="0"/>
+      <c r="SD1" s="0"/>
+      <c r="SE1" s="0"/>
+      <c r="SF1" s="0"/>
+      <c r="SG1" s="0"/>
+      <c r="SH1" s="0"/>
+      <c r="SI1" s="0"/>
+      <c r="SJ1" s="0"/>
+      <c r="SK1" s="0"/>
+      <c r="SL1" s="0"/>
+      <c r="SM1" s="0"/>
+      <c r="SN1" s="0"/>
+      <c r="SO1" s="0"/>
+      <c r="SP1" s="0"/>
+      <c r="SQ1" s="0"/>
+      <c r="SR1" s="0"/>
+      <c r="SS1" s="0"/>
+      <c r="ST1" s="0"/>
+      <c r="SU1" s="0"/>
+      <c r="SV1" s="0"/>
+      <c r="SW1" s="0"/>
+      <c r="SX1" s="0"/>
+      <c r="SY1" s="0"/>
+      <c r="SZ1" s="0"/>
+      <c r="TA1" s="0"/>
+      <c r="TB1" s="0"/>
+      <c r="TC1" s="0"/>
+      <c r="TD1" s="0"/>
+      <c r="TE1" s="0"/>
+      <c r="TF1" s="0"/>
+      <c r="TG1" s="0"/>
+      <c r="TH1" s="0"/>
+      <c r="TI1" s="0"/>
+      <c r="TJ1" s="0"/>
+      <c r="TK1" s="0"/>
+      <c r="TL1" s="0"/>
+      <c r="TM1" s="0"/>
+      <c r="TN1" s="0"/>
+      <c r="TO1" s="0"/>
+      <c r="TP1" s="0"/>
+      <c r="TQ1" s="0"/>
+      <c r="TR1" s="0"/>
+      <c r="TS1" s="0"/>
+      <c r="TT1" s="0"/>
+      <c r="TU1" s="0"/>
+      <c r="TV1" s="0"/>
+      <c r="TW1" s="0"/>
+      <c r="TX1" s="0"/>
+      <c r="TY1" s="0"/>
+      <c r="TZ1" s="0"/>
+      <c r="UA1" s="0"/>
+      <c r="UB1" s="0"/>
+      <c r="UC1" s="0"/>
+      <c r="UD1" s="0"/>
+      <c r="UE1" s="0"/>
+      <c r="UF1" s="0"/>
+      <c r="UG1" s="0"/>
+      <c r="UH1" s="0"/>
+      <c r="UI1" s="0"/>
+      <c r="UJ1" s="0"/>
+      <c r="UK1" s="0"/>
+      <c r="UL1" s="0"/>
+      <c r="UM1" s="0"/>
+      <c r="UN1" s="0"/>
+      <c r="UO1" s="0"/>
+      <c r="UP1" s="0"/>
+      <c r="UQ1" s="0"/>
+      <c r="UR1" s="0"/>
+      <c r="US1" s="0"/>
+      <c r="UT1" s="0"/>
+      <c r="UU1" s="0"/>
+      <c r="UV1" s="0"/>
+      <c r="UW1" s="0"/>
+      <c r="UX1" s="0"/>
+      <c r="UY1" s="0"/>
+      <c r="UZ1" s="0"/>
+      <c r="VA1" s="0"/>
+      <c r="VB1" s="0"/>
+      <c r="VC1" s="0"/>
+      <c r="VD1" s="0"/>
+      <c r="VE1" s="0"/>
+      <c r="VF1" s="0"/>
+      <c r="VG1" s="0"/>
+      <c r="VH1" s="0"/>
+      <c r="VI1" s="0"/>
+      <c r="VJ1" s="0"/>
+      <c r="VK1" s="0"/>
+      <c r="VL1" s="0"/>
+      <c r="VM1" s="0"/>
+      <c r="VN1" s="0"/>
+      <c r="VO1" s="0"/>
+      <c r="VP1" s="0"/>
+      <c r="VQ1" s="0"/>
+      <c r="VR1" s="0"/>
+      <c r="VS1" s="0"/>
+      <c r="VT1" s="0"/>
+      <c r="VU1" s="0"/>
+      <c r="VV1" s="0"/>
+      <c r="VW1" s="0"/>
+      <c r="VX1" s="0"/>
+      <c r="VY1" s="0"/>
+      <c r="VZ1" s="0"/>
+      <c r="WA1" s="0"/>
+      <c r="WB1" s="0"/>
+      <c r="WC1" s="0"/>
+      <c r="WD1" s="0"/>
+      <c r="WE1" s="0"/>
+      <c r="WF1" s="0"/>
+      <c r="WG1" s="0"/>
+      <c r="WH1" s="0"/>
+      <c r="WI1" s="0"/>
+      <c r="WJ1" s="0"/>
+      <c r="WK1" s="0"/>
+      <c r="WL1" s="0"/>
+      <c r="WM1" s="0"/>
+      <c r="WN1" s="0"/>
+      <c r="WO1" s="0"/>
+      <c r="WP1" s="0"/>
+      <c r="WQ1" s="0"/>
+      <c r="WR1" s="0"/>
+      <c r="WS1" s="0"/>
+      <c r="WT1" s="0"/>
+      <c r="WU1" s="0"/>
+      <c r="WV1" s="0"/>
+      <c r="WW1" s="0"/>
+      <c r="WX1" s="0"/>
+      <c r="WY1" s="0"/>
+      <c r="WZ1" s="0"/>
+      <c r="XA1" s="0"/>
+      <c r="XB1" s="0"/>
+      <c r="XC1" s="0"/>
+      <c r="XD1" s="0"/>
+      <c r="XE1" s="0"/>
+      <c r="XF1" s="0"/>
+      <c r="XG1" s="0"/>
+      <c r="XH1" s="0"/>
+      <c r="XI1" s="0"/>
+      <c r="XJ1" s="0"/>
+      <c r="XK1" s="0"/>
+      <c r="XL1" s="0"/>
+      <c r="XM1" s="0"/>
+      <c r="XN1" s="0"/>
+      <c r="XO1" s="0"/>
+      <c r="XP1" s="0"/>
+      <c r="XQ1" s="0"/>
+      <c r="XR1" s="0"/>
+      <c r="XS1" s="0"/>
+      <c r="XT1" s="0"/>
+      <c r="XU1" s="0"/>
+      <c r="XV1" s="0"/>
+      <c r="XW1" s="0"/>
+      <c r="XX1" s="0"/>
+      <c r="XY1" s="0"/>
+      <c r="XZ1" s="0"/>
+      <c r="YA1" s="0"/>
+      <c r="YB1" s="0"/>
+      <c r="YC1" s="0"/>
+      <c r="YD1" s="0"/>
+      <c r="YE1" s="0"/>
+      <c r="YF1" s="0"/>
+      <c r="YG1" s="0"/>
+      <c r="YH1" s="0"/>
+      <c r="YI1" s="0"/>
+      <c r="YJ1" s="0"/>
+      <c r="YK1" s="0"/>
+      <c r="YL1" s="0"/>
+      <c r="YM1" s="0"/>
+      <c r="YN1" s="0"/>
+      <c r="YO1" s="0"/>
+      <c r="YP1" s="0"/>
+      <c r="YQ1" s="0"/>
+      <c r="YR1" s="0"/>
+      <c r="YS1" s="0"/>
+      <c r="YT1" s="0"/>
+      <c r="YU1" s="0"/>
+      <c r="YV1" s="0"/>
+      <c r="YW1" s="0"/>
+      <c r="YX1" s="0"/>
+      <c r="YY1" s="0"/>
+      <c r="YZ1" s="0"/>
+      <c r="ZA1" s="0"/>
+      <c r="ZB1" s="0"/>
+      <c r="ZC1" s="0"/>
+      <c r="ZD1" s="0"/>
+      <c r="ZE1" s="0"/>
+      <c r="ZF1" s="0"/>
+      <c r="ZG1" s="0"/>
+      <c r="ZH1" s="0"/>
+      <c r="ZI1" s="0"/>
+      <c r="ZJ1" s="0"/>
+      <c r="ZK1" s="0"/>
+      <c r="ZL1" s="0"/>
+      <c r="ZM1" s="0"/>
+      <c r="ZN1" s="0"/>
+      <c r="ZO1" s="0"/>
+      <c r="ZP1" s="0"/>
+      <c r="ZQ1" s="0"/>
+      <c r="ZR1" s="0"/>
+      <c r="ZS1" s="0"/>
+      <c r="ZT1" s="0"/>
+      <c r="ZU1" s="0"/>
+      <c r="ZV1" s="0"/>
+      <c r="ZW1" s="0"/>
+      <c r="ZX1" s="0"/>
+      <c r="ZY1" s="0"/>
+      <c r="ZZ1" s="0"/>
+      <c r="AAA1" s="0"/>
+      <c r="AAB1" s="0"/>
+      <c r="AAC1" s="0"/>
+      <c r="AAD1" s="0"/>
+      <c r="AAE1" s="0"/>
+      <c r="AAF1" s="0"/>
+      <c r="AAG1" s="0"/>
+      <c r="AAH1" s="0"/>
+      <c r="AAI1" s="0"/>
+      <c r="AAJ1" s="0"/>
+      <c r="AAK1" s="0"/>
+      <c r="AAL1" s="0"/>
+      <c r="AAM1" s="0"/>
+      <c r="AAN1" s="0"/>
+      <c r="AAO1" s="0"/>
+      <c r="AAP1" s="0"/>
+      <c r="AAQ1" s="0"/>
+      <c r="AAR1" s="0"/>
+      <c r="AAS1" s="0"/>
+      <c r="AAT1" s="0"/>
+      <c r="AAU1" s="0"/>
+      <c r="AAV1" s="0"/>
+      <c r="AAW1" s="0"/>
+      <c r="AAX1" s="0"/>
+      <c r="AAY1" s="0"/>
+      <c r="AAZ1" s="0"/>
+      <c r="ABA1" s="0"/>
+      <c r="ABB1" s="0"/>
+      <c r="ABC1" s="0"/>
+      <c r="ABD1" s="0"/>
+      <c r="ABE1" s="0"/>
+      <c r="ABF1" s="0"/>
+      <c r="ABG1" s="0"/>
+      <c r="ABH1" s="0"/>
+      <c r="ABI1" s="0"/>
+      <c r="ABJ1" s="0"/>
+      <c r="ABK1" s="0"/>
+      <c r="ABL1" s="0"/>
+      <c r="ABM1" s="0"/>
+      <c r="ABN1" s="0"/>
+      <c r="ABO1" s="0"/>
+      <c r="ABP1" s="0"/>
+      <c r="ABQ1" s="0"/>
+      <c r="ABR1" s="0"/>
+      <c r="ABS1" s="0"/>
+      <c r="ABT1" s="0"/>
+      <c r="ABU1" s="0"/>
+      <c r="ABV1" s="0"/>
+      <c r="ABW1" s="0"/>
+      <c r="ABX1" s="0"/>
+      <c r="ABY1" s="0"/>
+      <c r="ABZ1" s="0"/>
+      <c r="ACA1" s="0"/>
+      <c r="ACB1" s="0"/>
+      <c r="ACC1" s="0"/>
+      <c r="ACD1" s="0"/>
+      <c r="ACE1" s="0"/>
+      <c r="ACF1" s="0"/>
+      <c r="ACG1" s="0"/>
+      <c r="ACH1" s="0"/>
+      <c r="ACI1" s="0"/>
+      <c r="ACJ1" s="0"/>
+      <c r="ACK1" s="0"/>
+      <c r="ACL1" s="0"/>
+      <c r="ACM1" s="0"/>
+      <c r="ACN1" s="0"/>
+      <c r="ACO1" s="0"/>
+      <c r="ACP1" s="0"/>
+      <c r="ACQ1" s="0"/>
+      <c r="ACR1" s="0"/>
+      <c r="ACS1" s="0"/>
+      <c r="ACT1" s="0"/>
+      <c r="ACU1" s="0"/>
+      <c r="ACV1" s="0"/>
+      <c r="ACW1" s="0"/>
+      <c r="ACX1" s="0"/>
+      <c r="ACY1" s="0"/>
+      <c r="ACZ1" s="0"/>
+      <c r="ADA1" s="0"/>
+      <c r="ADB1" s="0"/>
+      <c r="ADC1" s="0"/>
+      <c r="ADD1" s="0"/>
+      <c r="ADE1" s="0"/>
+      <c r="ADF1" s="0"/>
+      <c r="ADG1" s="0"/>
+      <c r="ADH1" s="0"/>
+      <c r="ADI1" s="0"/>
+      <c r="ADJ1" s="0"/>
+      <c r="ADK1" s="0"/>
+      <c r="ADL1" s="0"/>
+      <c r="ADM1" s="0"/>
+      <c r="ADN1" s="0"/>
+      <c r="ADO1" s="0"/>
+      <c r="ADP1" s="0"/>
+      <c r="ADQ1" s="0"/>
+      <c r="ADR1" s="0"/>
+      <c r="ADS1" s="0"/>
+      <c r="ADT1" s="0"/>
+      <c r="ADU1" s="0"/>
+      <c r="ADV1" s="0"/>
+      <c r="ADW1" s="0"/>
+      <c r="ADX1" s="0"/>
+      <c r="ADY1" s="0"/>
+      <c r="ADZ1" s="0"/>
+      <c r="AEA1" s="0"/>
+      <c r="AEB1" s="0"/>
+      <c r="AEC1" s="0"/>
+      <c r="AED1" s="0"/>
+      <c r="AEE1" s="0"/>
+      <c r="AEF1" s="0"/>
+      <c r="AEG1" s="0"/>
+      <c r="AEH1" s="0"/>
+      <c r="AEI1" s="0"/>
+      <c r="AEJ1" s="0"/>
+      <c r="AEK1" s="0"/>
+      <c r="AEL1" s="0"/>
+      <c r="AEM1" s="0"/>
+      <c r="AEN1" s="0"/>
+      <c r="AEO1" s="0"/>
+      <c r="AEP1" s="0"/>
+      <c r="AEQ1" s="0"/>
+      <c r="AER1" s="0"/>
+      <c r="AES1" s="0"/>
+      <c r="AET1" s="0"/>
+      <c r="AEU1" s="0"/>
+      <c r="AEV1" s="0"/>
+      <c r="AEW1" s="0"/>
+      <c r="AEX1" s="0"/>
+      <c r="AEY1" s="0"/>
+      <c r="AEZ1" s="0"/>
+      <c r="AFA1" s="0"/>
+      <c r="AFB1" s="0"/>
+      <c r="AFC1" s="0"/>
+      <c r="AFD1" s="0"/>
+      <c r="AFE1" s="0"/>
+      <c r="AFF1" s="0"/>
+      <c r="AFG1" s="0"/>
+      <c r="AFH1" s="0"/>
+      <c r="AFI1" s="0"/>
+      <c r="AFJ1" s="0"/>
+      <c r="AFK1" s="0"/>
+      <c r="AFL1" s="0"/>
+      <c r="AFM1" s="0"/>
+      <c r="AFN1" s="0"/>
+      <c r="AFO1" s="0"/>
+      <c r="AFP1" s="0"/>
+      <c r="AFQ1" s="0"/>
+      <c r="AFR1" s="0"/>
+      <c r="AFS1" s="0"/>
+      <c r="AFT1" s="0"/>
+      <c r="AFU1" s="0"/>
+      <c r="AFV1" s="0"/>
+      <c r="AFW1" s="0"/>
+      <c r="AFX1" s="0"/>
+      <c r="AFY1" s="0"/>
+      <c r="AFZ1" s="0"/>
+      <c r="AGA1" s="0"/>
+      <c r="AGB1" s="0"/>
+      <c r="AGC1" s="0"/>
+      <c r="AGD1" s="0"/>
+      <c r="AGE1" s="0"/>
+      <c r="AGF1" s="0"/>
+      <c r="AGG1" s="0"/>
+      <c r="AGH1" s="0"/>
+      <c r="AGI1" s="0"/>
+      <c r="AGJ1" s="0"/>
+      <c r="AGK1" s="0"/>
+      <c r="AGL1" s="0"/>
+      <c r="AGM1" s="0"/>
+      <c r="AGN1" s="0"/>
+      <c r="AGO1" s="0"/>
+      <c r="AGP1" s="0"/>
+      <c r="AGQ1" s="0"/>
+      <c r="AGR1" s="0"/>
+      <c r="AGS1" s="0"/>
+      <c r="AGT1" s="0"/>
+      <c r="AGU1" s="0"/>
+      <c r="AGV1" s="0"/>
+      <c r="AGW1" s="0"/>
+      <c r="AGX1" s="0"/>
+      <c r="AGY1" s="0"/>
+      <c r="AGZ1" s="0"/>
+      <c r="AHA1" s="0"/>
+      <c r="AHB1" s="0"/>
+      <c r="AHC1" s="0"/>
+      <c r="AHD1" s="0"/>
+      <c r="AHE1" s="0"/>
+      <c r="AHF1" s="0"/>
+      <c r="AHG1" s="0"/>
+      <c r="AHH1" s="0"/>
+      <c r="AHI1" s="0"/>
+      <c r="AHJ1" s="0"/>
+      <c r="AHK1" s="0"/>
+      <c r="AHL1" s="0"/>
+      <c r="AHM1" s="0"/>
+      <c r="AHN1" s="0"/>
+      <c r="AHO1" s="0"/>
+      <c r="AHP1" s="0"/>
+      <c r="AHQ1" s="0"/>
+      <c r="AHR1" s="0"/>
+      <c r="AHS1" s="0"/>
+      <c r="AHT1" s="0"/>
+      <c r="AHU1" s="0"/>
+      <c r="AHV1" s="0"/>
+      <c r="AHW1" s="0"/>
+      <c r="AHX1" s="0"/>
+      <c r="AHY1" s="0"/>
+      <c r="AHZ1" s="0"/>
+      <c r="AIA1" s="0"/>
+      <c r="AIB1" s="0"/>
+      <c r="AIC1" s="0"/>
+      <c r="AID1" s="0"/>
+      <c r="AIE1" s="0"/>
+      <c r="AIF1" s="0"/>
+      <c r="AIG1" s="0"/>
+      <c r="AIH1" s="0"/>
+      <c r="AII1" s="0"/>
+      <c r="AIJ1" s="0"/>
+      <c r="AIK1" s="0"/>
+      <c r="AIL1" s="0"/>
+      <c r="AIM1" s="0"/>
+      <c r="AIN1" s="0"/>
+      <c r="AIO1" s="0"/>
+      <c r="AIP1" s="0"/>
+      <c r="AIQ1" s="0"/>
+      <c r="AIR1" s="0"/>
+      <c r="AIS1" s="0"/>
+      <c r="AIT1" s="0"/>
+      <c r="AIU1" s="0"/>
+      <c r="AIV1" s="0"/>
+      <c r="AIW1" s="0"/>
+      <c r="AIX1" s="0"/>
+      <c r="AIY1" s="0"/>
+      <c r="AIZ1" s="0"/>
+      <c r="AJA1" s="0"/>
+      <c r="AJB1" s="0"/>
+      <c r="AJC1" s="0"/>
+      <c r="AJD1" s="0"/>
+      <c r="AJE1" s="0"/>
+      <c r="AJF1" s="0"/>
+      <c r="AJG1" s="0"/>
+      <c r="AJH1" s="0"/>
+      <c r="AJI1" s="0"/>
+      <c r="AJJ1" s="0"/>
+      <c r="AJK1" s="0"/>
+      <c r="AJL1" s="0"/>
+      <c r="AJM1" s="0"/>
+      <c r="AJN1" s="0"/>
+      <c r="AJO1" s="0"/>
+      <c r="AJP1" s="0"/>
+      <c r="AJQ1" s="0"/>
+      <c r="AJR1" s="0"/>
+      <c r="AJS1" s="0"/>
+      <c r="AJT1" s="0"/>
+      <c r="AJU1" s="0"/>
+      <c r="AJV1" s="0"/>
+      <c r="AJW1" s="0"/>
+      <c r="AJX1" s="0"/>
+      <c r="AJY1" s="0"/>
+      <c r="AJZ1" s="0"/>
+      <c r="AKA1" s="0"/>
+      <c r="AKB1" s="0"/>
+      <c r="AKC1" s="0"/>
+      <c r="AKD1" s="0"/>
+      <c r="AKE1" s="0"/>
+      <c r="AKF1" s="0"/>
+      <c r="AKG1" s="0"/>
+      <c r="AKH1" s="0"/>
+      <c r="AKI1" s="0"/>
+      <c r="AKJ1" s="0"/>
+      <c r="AKK1" s="0"/>
+      <c r="AKL1" s="0"/>
+      <c r="AKM1" s="0"/>
+      <c r="AKN1" s="0"/>
+      <c r="AKO1" s="0"/>
+      <c r="AKP1" s="0"/>
+      <c r="AKQ1" s="0"/>
+      <c r="AKR1" s="0"/>
+      <c r="AKS1" s="0"/>
+      <c r="AKT1" s="0"/>
+      <c r="AKU1" s="0"/>
+      <c r="AKV1" s="0"/>
+      <c r="AKW1" s="0"/>
+      <c r="AKX1" s="0"/>
+      <c r="AKY1" s="0"/>
+      <c r="AKZ1" s="0"/>
+      <c r="ALA1" s="0"/>
+      <c r="ALB1" s="0"/>
+      <c r="ALC1" s="0"/>
+      <c r="ALD1" s="0"/>
+      <c r="ALE1" s="0"/>
+      <c r="ALF1" s="0"/>
+      <c r="ALG1" s="0"/>
+      <c r="ALH1" s="0"/>
+      <c r="ALI1" s="0"/>
+      <c r="ALJ1" s="0"/>
+      <c r="ALK1" s="0"/>
+      <c r="ALL1" s="0"/>
+      <c r="ALM1" s="0"/>
+      <c r="ALN1" s="0"/>
+      <c r="ALO1" s="0"/>
+      <c r="ALP1" s="0"/>
+      <c r="ALQ1" s="0"/>
+      <c r="ALR1" s="0"/>
+      <c r="ALS1" s="0"/>
+      <c r="ALT1" s="0"/>
+      <c r="ALU1" s="0"/>
+      <c r="ALV1" s="0"/>
+      <c r="ALW1" s="0"/>
+      <c r="ALX1" s="0"/>
+      <c r="ALY1" s="0"/>
+      <c r="ALZ1" s="0"/>
+      <c r="AMA1" s="0"/>
+      <c r="AMB1" s="0"/>
+      <c r="AMC1" s="0"/>
+      <c r="AMD1" s="0"/>
+      <c r="AME1" s="0"/>
+      <c r="AMF1" s="0"/>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" s="5" customFormat="true" ht="82.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
@@ -560,11 +1577,11 @@
         <v>5</v>
       </c>
       <c r="G3" s="8" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H3" s="9" t="n">
         <f aca="false">+F3*G3</f>
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>14</v>
@@ -593,11 +1610,11 @@
         <v>3</v>
       </c>
       <c r="G4" s="8" t="n">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="H4" s="9" t="n">
         <f aca="false">+F4*G4</f>
-        <v>1.5</v>
+        <v>0.3</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>18</v>
@@ -666,10 +1683,10 @@
         <v>0.2</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" s="11" customFormat="true" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -680,10 +1697,10 @@
         <v>42098</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>13</v>
@@ -692,17 +1709,17 @@
         <v>3</v>
       </c>
       <c r="G7" s="8" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H7" s="9" t="n">
         <f aca="false">+F7*G7</f>
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" s="11" customFormat="true" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -713,10 +1730,10 @@
         <v>42229</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>13</v>
@@ -725,17 +1742,17 @@
         <v>4</v>
       </c>
       <c r="G8" s="8" t="n">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="H8" s="9" t="n">
         <f aca="false">+F8*G8</f>
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" s="11" customFormat="true" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -746,10 +1763,10 @@
         <v>42229</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>13</v>
@@ -758,17 +1775,17 @@
         <v>5</v>
       </c>
       <c r="G9" s="8" t="n">
-        <v>0.9</v>
+        <v>0.55</v>
       </c>
       <c r="H9" s="9" t="n">
         <f aca="false">+F9*G9</f>
-        <v>4.5</v>
+        <v>2.75</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Update Lista de Riscos
</commit_message>
<xml_diff>
--- a/planejamento/CM_Lista_riscos.xlsx
+++ b/planejamento/CM_Lista_riscos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tarcisio.d.silva\Documents\GitHub\cmproject\cmproject.git\planejamento\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\Github\cmproject\planejamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Riscos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -205,7 +205,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -292,9 +292,6 @@
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="90" wrapText="1"/>
@@ -340,6 +337,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -607,7 +607,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -645,7 +645,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -717,7 +717,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -869,38 +869,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.625" style="2"/>
-    <col min="2" max="2" width="15.625" style="2"/>
-    <col min="3" max="3" width="36.25" style="2"/>
-    <col min="4" max="4" width="37" style="2"/>
-    <col min="5" max="5" width="3.875" style="2"/>
-    <col min="6" max="6" width="3.625" style="2"/>
-    <col min="7" max="7" width="7.125" style="2"/>
-    <col min="8" max="8" width="4" style="2"/>
-    <col min="9" max="9" width="11.875" style="2"/>
-    <col min="10" max="10" width="37.375" style="2"/>
-    <col min="11" max="1025" width="9.375" style="2"/>
+    <col min="1" max="1" width="3.625" style="1"/>
+    <col min="2" max="2" width="15.625" style="1"/>
+    <col min="3" max="3" width="36.25" style="1"/>
+    <col min="4" max="4" width="37" style="1"/>
+    <col min="5" max="5" width="3.875" style="1"/>
+    <col min="6" max="6" width="3.625" style="1"/>
+    <col min="7" max="7" width="7.125" style="1"/>
+    <col min="8" max="8" width="4" style="1"/>
+    <col min="9" max="9" width="11.875" style="1"/>
+    <col min="10" max="10" width="37.375" style="1"/>
+    <col min="11" max="1025" width="9.375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="22.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
       <c r="K1"/>
       <c r="L1"/>
       <c r="M1"/>
@@ -1916,455 +1916,455 @@
       <c r="AMI1"/>
       <c r="AMJ1"/>
     </row>
-    <row r="2" spans="1:1024" s="5" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:1024" s="4" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:1024" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A3" s="6">
+    <row r="3" spans="1:1024" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>42079</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>5</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <v>0</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="8">
         <f t="shared" ref="H3:H20" si="0">+F3*G3</f>
         <v>0</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:1024" s="11" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
+    <row r="4" spans="1:1024" s="10" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>42084</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>3</v>
       </c>
-      <c r="G4" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="H4" s="9">
-        <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1024" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
-        <v>3</v>
-      </c>
-      <c r="B5" s="7">
-        <v>42116</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="6">
-        <v>2</v>
-      </c>
-      <c r="G5" s="8">
-        <v>0.6</v>
-      </c>
-      <c r="H5" s="9">
-        <f t="shared" si="0"/>
-        <v>1.2</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1024" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
-        <v>4</v>
-      </c>
-      <c r="B6" s="7">
-        <v>42117</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="6">
-        <v>4</v>
-      </c>
-      <c r="G6" s="8">
-        <v>0.05</v>
-      </c>
-      <c r="H6" s="9">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1024" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
-        <v>5</v>
-      </c>
-      <c r="B7" s="7">
-        <v>42098</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="6">
-        <v>3</v>
-      </c>
-      <c r="G7" s="8">
+      <c r="G4" s="7">
         <v>0</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H4" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1024" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6">
+        <v>42116</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="5">
+        <v>2</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="H5" s="8">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J7" s="10" t="s">
-        <v>29</v>
+      <c r="J5" s="9" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:1024" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
-        <v>6</v>
-      </c>
-      <c r="B8" s="7">
-        <v>42229</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="6" t="s">
+    <row r="6" spans="1:1024" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6">
+        <v>42117</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F6" s="5">
         <v>4</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G6" s="7">
         <v>0</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H6" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1024" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6">
+        <v>42098</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="5">
+        <v>3</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1024" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6">
+        <v>42229</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="5">
+        <v>4</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0</v>
+      </c>
+      <c r="H8" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:1024" s="11" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
+    <row r="9" spans="1:1024" s="10" customFormat="1" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
         <v>7</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>42229</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>5</v>
       </c>
-      <c r="G9" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="H9" s="9">
+      <c r="G9" s="7">
+        <v>0</v>
+      </c>
+      <c r="H9" s="8">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="I9" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J9" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:1024" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>8</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="9">
+      <c r="B10" s="6"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I10" s="9"/>
-      <c r="J10" s="10"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="9"/>
     </row>
     <row r="11" spans="1:1024" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
+      <c r="A11" s="5">
         <v>9</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="9">
+      <c r="B11" s="6"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I11" s="9"/>
-      <c r="J11" s="10"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="9"/>
     </row>
     <row r="12" spans="1:1024" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
+      <c r="A12" s="5">
         <v>10</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="9">
+      <c r="B12" s="6"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I12" s="9"/>
-      <c r="J12" s="10"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="9"/>
     </row>
     <row r="13" spans="1:1024" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
+      <c r="A13" s="5">
         <v>11</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="9">
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I13" s="16"/>
-      <c r="J13" s="17"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="16"/>
     </row>
     <row r="14" spans="1:1024" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
+      <c r="A14" s="5">
         <v>12</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="9">
+      <c r="B14" s="6"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I14" s="9"/>
-      <c r="J14" s="10"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="9"/>
     </row>
     <row r="15" spans="1:1024" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
+      <c r="A15" s="5">
         <v>13</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="9">
+      <c r="B15" s="6"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I15" s="9"/>
-      <c r="J15" s="10"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="9"/>
     </row>
     <row r="16" spans="1:1024" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="6">
+      <c r="A16" s="5">
         <v>14</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="9">
+      <c r="B16" s="6"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I16" s="9"/>
-      <c r="J16" s="10"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="9"/>
     </row>
     <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="6">
+      <c r="A17" s="5">
         <v>15</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="9">
+      <c r="B17" s="6"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I17" s="9"/>
-      <c r="J17" s="6"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="6">
+      <c r="A18" s="5">
         <v>16</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="9">
+      <c r="B18" s="6"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I18" s="9"/>
-      <c r="J18" s="6"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="6">
+      <c r="A19" s="5">
         <v>17</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="9">
+      <c r="B19" s="6"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I19" s="9"/>
-      <c r="J19" s="6"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="5"/>
     </row>
     <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="6">
+      <c r="A20" s="5">
         <v>18</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="9">
+      <c r="B20" s="6"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I20" s="9"/>
-      <c r="J20" s="6"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="5"/>
     </row>
     <row r="26" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>

</xml_diff>